<commit_message>
Modif en BD: Nueva tabla, sector ABM sector Nueva operacion: consulta info personas
</commit_message>
<xml_diff>
--- a/archivos/02 - Querys Insert entidades, personas/Datos entidades, personas.xlsx
+++ b/archivos/02 - Querys Insert entidades, personas/Datos entidades, personas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="4" windowWidth="19200" windowHeight="8330"/>
+    <workbookView activeTab="1" windowWidth="12460" windowHeight="4700"/>
   </bookViews>
   <sheets>
     <sheet name="entidad" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57" count="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52" count="52">
   <si>
     <t>ID</t>
   </si>
@@ -57,25 +57,28 @@
     <t>INSERT INTO sgr.entidad ( id_entidad, razonsocial, cuit, fbaja, propietario ) VALUES (3,'SHOPPING A','31724561201',DEFAULT,'FALSE');</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (1,'1','ALMIRON','ALEJANDRO','1981-01-01','2','2','13','1','1','2',DEFAULT,'1','1','28214841');</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (1,'1','ALMIRON','ALEJANDRO','1981-01-01','2','29','1','1','2',DEFAULT,'1','1','28214841');</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (2,'1','BARBOZA','ARIEL','1982-02-02','2','2','13','1','1','1',DEFAULT,'1','1','28041320');</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (2,'1','BARBOZA','ARIEL','1982-02-02','2','28','1','1','1',DEFAULT,'1','1','28041320');</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (3,'1','PEDROZO','CRISTIAN','1983-03-03','2','2','13','3','1','1',DEFAULT,'1','1','36330420');</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (3,'1','PEDROZO','CRISTIAN','1983-03-03','2','27','3','1','1',DEFAULT,'1','1','36330420');</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (4,'2','AGUIRRE','AGUSTIN','1984-04-04','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'2','1472583');</t>
+    <t>NULL</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (5,'2','GUTIERREZ','LEANDRO','1985-05-05','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'3','258369');</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (4,'2','AGUIRRE','AGUSTIN','1984-04-04','2',NULL,NULL,'1','1',NULL,NULL,'2','1472583');</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sucursal, id_dpto, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (6,'2','GARCIA','TOMAS','1986-06-06','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'4','7412580');</t>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (5,'2','GUTIERREZ','LEANDRO','1985-05-05','2',NULL,NULL,'1','1',NULL,NULL,'3','258369');</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.persona ( id_persona, id_camposempleado, apellido, nombre, fnac, id_genero, id_sector, id_rol, id_nacionalidad, id_estadocivil, fbaja, id_entidad, id_tipo_doc, doc ) VALUES (6,'2','GARCIA','TOMAS','1986-06-06','2',NULL,NULL,'1','1',NULL,NULL,'4','7412580');</t>
   </si>
   <si>
     <t>num</t>
@@ -102,37 +105,19 @@
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (3,'Barrio uno','La primera','123','-','3',DEFAULT,'10053');</t>
   </si>
   <si>
-    <t>Los Alelies</t>
-  </si>
-  <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (4,'Santa Rosa','Los Alelies','1','-',DEFAULT,1,'10053');</t>
-  </si>
-  <si>
-    <t>Los Tulipanes</t>
   </si>
   <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (5,'Las Orquideas','Los Tulipanes','2','-',DEFAULT,2,'10053');</t>
   </si>
   <si>
-    <t>Av. Castelli</t>
-  </si>
-  <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (6,'San Martin','Av. Castelli','3','-',DEFAULT,3,'10053');</t>
-  </si>
-  <si>
-    <t>Los Cedros</t>
   </si>
   <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (7,'Villa Nueva','Los Cedros','4','-',DEFAULT,4,'10053');</t>
   </si>
   <si>
-    <t>Los lapachos</t>
-  </si>
-  <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (8,'Villa 14','Los lapachos','5','-',DEFAULT,5,'10053');</t>
-  </si>
-  <si>
-    <t>J. I. Rucci</t>
   </si>
   <si>
     <t>INSERT INTO sgr.domicilio ( id_domicilio, barrio, calle, num, piso, id_entidad, id_persona, id_ciudad )  VALUES (9,'Belen','J. I. Rucci','6','-',DEFAULT,6,'10053');</t>
@@ -16882,10 +16867,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75">
-      <selection activeCell="W2" sqref="W2:W7"/>
+    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+      <selection activeCell="V2" sqref="V2:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16896,17 +16881,18 @@
     <col min="4" max="4" style="1" width="9.142307692307693"/>
     <col min="5" max="5" style="1" width="13.522996794871796" customWidth="1"/>
     <col min="6" max="6" style="1" width="8.95184294871795" customWidth="1"/>
-    <col min="7" max="9" style="1" width="9.142307692307693"/>
-    <col min="10" max="10" style="1" width="12.42782451923077" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" style="1" width="9.142307692307693"/>
-    <col min="14" max="16" style="1" width="12.142127403846155" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" style="1" width="9.142307692307693"/>
-    <col min="19" max="19" style="1" width="94.66097756410258" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" style="1" width="9.856550480769231" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" style="1" width="9.142307692307693"/>
+    <col min="7" max="8" style="1" width="9.142307692307693"/>
+    <col min="9" max="9" style="1" width="12.42782451923077" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" style="1" width="9.142307692307693"/>
+    <col min="13" max="15" style="1" width="12.142127403846155" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" style="1" width="9.142307692307693"/>
+    <col min="18" max="18" style="1" width="94.66097756410258" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" style="1" width="9.856550480769231" bestFit="1" customWidth="1"/>
+    <col min="20" max="16383" style="1" width="9.142307692307693"/>
+    <col min="16384" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384">
+    <row r="1" spans="1:16383">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16937,49 +16923,44 @@
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>id_sucursal</t>
+          <t>id_sector</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>id_dpto</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>id_rol</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>id_nacionalidad</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>id_estadocivil</t>
         </is>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>id_entidad</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>id_tipo_doc</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>doc</t>
         </is>
       </c>
     </row>
-    <row r="2" spans="1:16384">
+    <row r="2" spans="1:16383">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17005,48 +16986,45 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="H2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2">
         <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
         <v>28214841</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Q2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" t="str">
-        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;"'"&amp;F2&amp;"'"&amp;","&amp;"'"&amp;G2&amp;"'"&amp;","&amp;"'"&amp;H2&amp;"'"&amp;","&amp;"'"&amp;I2&amp;"'"&amp;","&amp;"'"&amp;J2&amp;"'"&amp;","&amp;"'"&amp;K2&amp;"'"&amp;","&amp;L2&amp;","&amp;"'"&amp;M2&amp;"'"&amp;","&amp;"'"&amp;N2&amp;"'"&amp;","&amp;"'"&amp;O2&amp;"'"&amp;")"</f>
-        <v>1,'1','ALMIRON','ALEJANDRO','1981-01-01','2','2','13','1','1','2',DEFAULT,'1','1','28214841')</v>
-      </c>
-      <c r="U2" t="s">
-        <f>R2&amp;S2&amp;";"</f>
+      <c r="R2" t="str">
+        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;"'"&amp;F2&amp;"'"&amp;","&amp;"'"&amp;G2&amp;"'"&amp;","&amp;"'"&amp;H2&amp;"'"&amp;","&amp;"'"&amp;I2&amp;"'"&amp;","&amp;"'"&amp;J2&amp;"'"&amp;","&amp;K2&amp;","&amp;"'"&amp;L2&amp;"'"&amp;","&amp;"'"&amp;M2&amp;"'"&amp;","&amp;"'"&amp;N2&amp;"'"&amp;")"</f>
+        <v>1,'1','ALMIRON','ALEJANDRO','1981-01-01','2','29','1','1','2',DEFAULT,'1','1','28214841')</v>
+      </c>
+      <c r="T2" t="s">
+        <f>Q2&amp;R2&amp;";"</f>
         <v>9</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16384">
+    <row r="3" spans="1:16383">
       <c r="A3">
         <v>2</v>
       </c>
@@ -17072,10 +17050,10 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -17083,37 +17061,34 @@
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3">
         <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
         <v>28041320</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q3" t="s">
         <v>8</v>
       </c>
-      <c r="S3" t="str">
-        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;"'"&amp;F3&amp;"'"&amp;","&amp;"'"&amp;G3&amp;"'"&amp;","&amp;"'"&amp;H3&amp;"'"&amp;","&amp;"'"&amp;I3&amp;"'"&amp;","&amp;"'"&amp;J3&amp;"'"&amp;","&amp;"'"&amp;K3&amp;"'"&amp;","&amp;L3&amp;","&amp;"'"&amp;M3&amp;"'"&amp;","&amp;"'"&amp;N3&amp;"'"&amp;","&amp;"'"&amp;O3&amp;"'"&amp;")"</f>
-        <v>2,'1','BARBOZA','ARIEL','1982-02-02','2','2','13','1','1','1',DEFAULT,'1','1','28041320')</v>
-      </c>
-      <c r="U3" t="s">
-        <f>R3&amp;S3&amp;";"</f>
+      <c r="R3" t="str">
+        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;"'"&amp;F3&amp;"'"&amp;","&amp;"'"&amp;G3&amp;"'"&amp;","&amp;"'"&amp;H3&amp;"'"&amp;","&amp;"'"&amp;I3&amp;"'"&amp;","&amp;"'"&amp;J3&amp;"'"&amp;","&amp;K3&amp;","&amp;"'"&amp;L3&amp;"'"&amp;","&amp;"'"&amp;M3&amp;"'"&amp;","&amp;"'"&amp;N3&amp;"'"&amp;")"</f>
+        <v>2,'1','BARBOZA','ARIEL','1982-02-02','2','28','1','1','1',DEFAULT,'1','1','28041320')</v>
+      </c>
+      <c r="T3" t="s">
+        <f>Q3&amp;R3&amp;";"</f>
         <v>10</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16383">
       <c r="A4">
         <v>3</v>
       </c>
@@ -17139,48 +17114,45 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4">
         <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>2</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
         <v>36330420</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Q4" t="s">
         <v>8</v>
       </c>
-      <c r="S4" t="str">
-        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;"'"&amp;F4&amp;"'"&amp;","&amp;"'"&amp;G4&amp;"'"&amp;","&amp;"'"&amp;H4&amp;"'"&amp;","&amp;"'"&amp;I4&amp;"'"&amp;","&amp;"'"&amp;J4&amp;"'"&amp;","&amp;"'"&amp;K4&amp;"'"&amp;","&amp;L4&amp;","&amp;"'"&amp;M4&amp;"'"&amp;","&amp;"'"&amp;N4&amp;"'"&amp;","&amp;"'"&amp;O4&amp;"'"&amp;")"</f>
-        <v>3,'1','PEDROZO','CRISTIAN','1983-03-03','2','2','13','3','1','1',DEFAULT,'1','1','36330420')</v>
-      </c>
-      <c r="U4" t="s">
-        <f>R4&amp;S4&amp;";"</f>
+      <c r="R4" t="str">
+        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;"'"&amp;F4&amp;"'"&amp;","&amp;"'"&amp;G4&amp;"'"&amp;","&amp;"'"&amp;H4&amp;"'"&amp;","&amp;"'"&amp;I4&amp;"'"&amp;","&amp;"'"&amp;J4&amp;"'"&amp;","&amp;K4&amp;","&amp;"'"&amp;L4&amp;"'"&amp;","&amp;"'"&amp;M4&amp;"'"&amp;","&amp;"'"&amp;N4&amp;"'"&amp;")"</f>
+        <v>3,'1','PEDROZO','CRISTIAN','1983-03-03','2','27','3','1','1',DEFAULT,'1','1','36330420')</v>
+      </c>
+      <c r="T4" t="s">
+        <f>Q4&amp;R4&amp;";"</f>
         <v>11</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16383">
       <c r="A5">
         <v>4</v>
       </c>
@@ -17205,49 +17177,46 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5">
-        <v>2</v>
+      <c r="G5" t="s">
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5">
-        <v>1</v>
+      <c r="K5" t="s">
+        <v>12</v>
       </c>
       <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="M5" t="s">
-        <v>2</v>
-      </c>
       <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
         <v>1472583</v>
       </c>
-      <c r="R5" t="s">
+      <c r="Q5" t="s">
         <v>8</v>
       </c>
-      <c r="S5" t="str">
-        <f>A5&amp;","&amp;"'"&amp;B5&amp;"'"&amp;","&amp;"'"&amp;C5&amp;"'"&amp;","&amp;"'"&amp;D5&amp;"'"&amp;","&amp;"'"&amp;E5&amp;"'"&amp;","&amp;"'"&amp;F5&amp;"'"&amp;","&amp;"'"&amp;G5&amp;"'"&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;"'"&amp;J5&amp;"'"&amp;","&amp;"'"&amp;K5&amp;"'"&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;"'"&amp;N5&amp;"'"&amp;","&amp;"'"&amp;O5&amp;"'"&amp;")"</f>
-        <v>4,'2','AGUIRRE','AGUSTIN','1984-04-04','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'2','1472583')</v>
-      </c>
-      <c r="U5" t="s">
-        <f>R5&amp;S5&amp;";"</f>
-        <v>12</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>12</v>
+      <c r="R5" t="str">
+        <f>A5&amp;","&amp;"'"&amp;B5&amp;"'"&amp;","&amp;"'"&amp;C5&amp;"'"&amp;","&amp;"'"&amp;D5&amp;"'"&amp;","&amp;"'"&amp;E5&amp;"'"&amp;","&amp;"'"&amp;F5&amp;"'"&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;"'"&amp;I5&amp;"'"&amp;","&amp;"'"&amp;J5&amp;"'"&amp;","&amp;K5&amp;","&amp;L5&amp;","&amp;"'"&amp;M5&amp;"'"&amp;","&amp;"'"&amp;N5&amp;"'"&amp;")"</f>
+        <v>4,'2','AGUIRRE','AGUSTIN','1984-04-04','2',NULL,NULL,'1','1',NULL,NULL,'2','1472583')</v>
+      </c>
+      <c r="T5" t="s">
+        <f>Q5&amp;R5&amp;";"</f>
+        <v>13</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16383">
       <c r="A6">
         <v>5</v>
       </c>
@@ -17272,49 +17241,46 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>2</v>
+      <c r="G6" t="s">
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6">
-        <v>1</v>
+      <c r="K6" t="s">
+        <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6">
         <v>258369</v>
       </c>
-      <c r="R6" t="s">
+      <c r="Q6" t="s">
         <v>8</v>
       </c>
-      <c r="S6" t="str">
-        <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;"'"&amp;C6&amp;"'"&amp;","&amp;"'"&amp;D6&amp;"'"&amp;","&amp;"'"&amp;E6&amp;"'"&amp;","&amp;"'"&amp;F6&amp;"'"&amp;","&amp;"'"&amp;G6&amp;"'"&amp;","&amp;H6&amp;","&amp;I6&amp;","&amp;"'"&amp;J6&amp;"'"&amp;","&amp;"'"&amp;K6&amp;"'"&amp;","&amp;L6&amp;","&amp;M6&amp;","&amp;"'"&amp;N6&amp;"'"&amp;","&amp;"'"&amp;O6&amp;"'"&amp;")"</f>
-        <v>5,'2','GUTIERREZ','LEANDRO','1985-05-05','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'3','258369')</v>
-      </c>
-      <c r="U6" t="s">
-        <f>R6&amp;S6&amp;";"</f>
-        <v>13</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>13</v>
+      <c r="R6" t="str">
+        <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;"'"&amp;C6&amp;"'"&amp;","&amp;"'"&amp;D6&amp;"'"&amp;","&amp;"'"&amp;E6&amp;"'"&amp;","&amp;"'"&amp;F6&amp;"'"&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;"'"&amp;I6&amp;"'"&amp;","&amp;"'"&amp;J6&amp;"'"&amp;","&amp;K6&amp;","&amp;L6&amp;","&amp;"'"&amp;M6&amp;"'"&amp;","&amp;"'"&amp;N6&amp;"'"&amp;")"</f>
+        <v>5,'2','GUTIERREZ','LEANDRO','1985-05-05','2',NULL,NULL,'1','1',NULL,NULL,'3','258369')</v>
+      </c>
+      <c r="T6" t="s">
+        <f>Q6&amp;R6&amp;";"</f>
+        <v>14</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16383">
       <c r="A7">
         <v>6</v>
       </c>
@@ -17339,49 +17305,46 @@
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>2</v>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7">
-        <v>1</v>
+      <c r="K7" t="s">
+        <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
       </c>
       <c r="N7">
-        <v>4</v>
-      </c>
-      <c r="O7">
         <v>7412580</v>
       </c>
-      <c r="R7" t="s">
+      <c r="Q7" t="s">
         <v>8</v>
       </c>
-      <c r="S7" t="str">
-        <f>A7&amp;","&amp;"'"&amp;B7&amp;"'"&amp;","&amp;"'"&amp;C7&amp;"'"&amp;","&amp;"'"&amp;D7&amp;"'"&amp;","&amp;"'"&amp;E7&amp;"'"&amp;","&amp;"'"&amp;F7&amp;"'"&amp;","&amp;"'"&amp;G7&amp;"'"&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;"'"&amp;J7&amp;"'"&amp;","&amp;"'"&amp;K7&amp;"'"&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;"'"&amp;N7&amp;"'"&amp;","&amp;"'"&amp;O7&amp;"'"&amp;")"</f>
-        <v>6,'2','GARCIA','TOMAS','1986-06-06','2','2',DEFAULT,DEFAULT,'1','1',DEFAULT,DEFAULT,'4','7412580')</v>
-      </c>
-      <c r="U7" t="s">
-        <f>R7&amp;S7&amp;";"</f>
-        <v>14</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>14</v>
+      <c r="R7" t="str">
+        <f>A7&amp;","&amp;"'"&amp;B7&amp;"'"&amp;","&amp;"'"&amp;C7&amp;"'"&amp;","&amp;"'"&amp;D7&amp;"'"&amp;","&amp;"'"&amp;E7&amp;"'"&amp;","&amp;"'"&amp;F7&amp;"'"&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;"'"&amp;I7&amp;"'"&amp;","&amp;"'"&amp;J7&amp;"'"&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;"'"&amp;M7&amp;"'"&amp;","&amp;"'"&amp;N7&amp;"'"&amp;")"</f>
+        <v>6,'2','GARCIA','TOMAS','1986-06-06','2',NULL,NULL,'1','1',NULL,NULL,'4','7412580')</v>
+      </c>
+      <c r="T7" t="s">
+        <f>Q7&amp;R7&amp;";"</f>
+        <v>15</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:16383">
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
       <c r="I12" s="0"/>
@@ -17392,9 +17355,8 @@
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
       <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
     </row>
-    <row r="13" spans="1:16384">
+    <row r="13" spans="1:16383">
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
@@ -17408,9 +17370,8 @@
       <c r="Q13" s="0"/>
       <c r="R13" s="0"/>
       <c r="S13" s="0"/>
-      <c r="T13" s="0"/>
     </row>
-    <row r="1048575" spans="1:16384">
+    <row r="1048575" spans="1:16383">
       <c r="A1048575" s="0"/>
       <c r="B1048575" s="0"/>
       <c r="C1048575" s="0"/>
@@ -17433,9 +17394,8 @@
       <c r="T1048575" s="0"/>
       <c r="U1048575" s="0"/>
       <c r="V1048575" s="0"/>
-      <c r="W1048575" s="0"/>
     </row>
-    <row r="1048576" spans="1:16384">
+    <row r="1048576" spans="1:16383">
       <c r="A1048576" s="0"/>
       <c r="B1048576" s="0"/>
       <c r="C1048576" s="0"/>
@@ -33819,7 +33779,6 @@
       <c r="XFA1048576" s="0"/>
       <c r="XFB1048576" s="0"/>
       <c r="XFC1048576" s="0"/>
-      <c r="XFD1048576" s="0"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -33869,7 +33828,7 @@
         </is>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
@@ -33877,10 +33836,10 @@
         </is>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
@@ -33926,7 +33885,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;"'"&amp;F2&amp;"'"&amp;","&amp;G2&amp;","&amp;"'"&amp;H2&amp;"'"&amp;")"</f>
@@ -33935,11 +33894,11 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <f>J2&amp;K2&amp;";"</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.25">
@@ -33957,10 +33916,10 @@
         </is>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -33973,7 +33932,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="1" t="str">
         <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;"'"&amp;F3&amp;"'"&amp;","&amp;G3&amp;","&amp;"'"&amp;H3&amp;"'"&amp;")"</f>
@@ -33982,11 +33941,11 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.25">
@@ -34007,7 +33966,7 @@
         <v>123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -34020,7 +33979,7 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="1" t="str">
         <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;"'"&amp;F4&amp;"'"&amp;","&amp;G4&amp;","&amp;"'"&amp;H4&amp;"'"&amp;")"</f>
@@ -34029,11 +33988,11 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
         <f>J4&amp;K4&amp;";"</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.25">
@@ -34045,14 +34004,16 @@
           <t>Santa Rosa</t>
         </is>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Los Alelies</t>
+        </is>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>2</v>
@@ -34064,7 +34025,7 @@
         <v>10053</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1" t="str">
         <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;"'"&amp;C6&amp;"'"&amp;","&amp;"'"&amp;D6&amp;"'"&amp;","&amp;"'"&amp;E6&amp;"'"&amp;","&amp;F6&amp;","&amp;G6&amp;","&amp;"'"&amp;H6&amp;"'"&amp;")"</f>
@@ -34089,14 +34050,16 @@
           <t>Las Orquideas</t>
         </is>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Los Tulipanes</t>
+        </is>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
@@ -34108,7 +34071,7 @@
         <v>10053</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1" t="str">
         <f>A7&amp;","&amp;"'"&amp;B7&amp;"'"&amp;","&amp;"'"&amp;C7&amp;"'"&amp;","&amp;"'"&amp;D7&amp;"'"&amp;","&amp;"'"&amp;E7&amp;"'"&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;"'"&amp;H7&amp;"'"&amp;")"</f>
@@ -34117,11 +34080,11 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
         <f>J7&amp;K7&amp;";"</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="14.25">
@@ -34133,14 +34096,16 @@
           <t>San Martin</t>
         </is>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Av. Castelli</t>
+        </is>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>2</v>
@@ -34152,7 +34117,7 @@
         <v>10053</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K8" s="1" t="str">
         <f>A8&amp;","&amp;"'"&amp;B8&amp;"'"&amp;","&amp;"'"&amp;C8&amp;"'"&amp;","&amp;"'"&amp;D8&amp;"'"&amp;","&amp;"'"&amp;E8&amp;"'"&amp;","&amp;F8&amp;","&amp;G8&amp;","&amp;"'"&amp;H8&amp;"'"&amp;")"</f>
@@ -34161,11 +34126,11 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
         <f>J8&amp;K8&amp;";"</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="14.25">
@@ -34177,14 +34142,16 @@
           <t>Villa Nueva</t>
         </is>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Los Cedros</t>
+        </is>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>2</v>
@@ -34196,7 +34163,7 @@
         <v>10053</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K9" s="1" t="str">
         <f>A9&amp;","&amp;"'"&amp;B9&amp;"'"&amp;","&amp;"'"&amp;C9&amp;"'"&amp;","&amp;"'"&amp;D9&amp;"'"&amp;","&amp;"'"&amp;E9&amp;"'"&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;"'"&amp;H9&amp;"'"&amp;")"</f>
@@ -34205,11 +34172,11 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
         <f>J9&amp;K9&amp;";"</f>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.25">
@@ -34221,14 +34188,16 @@
           <t>Villa 14</t>
         </is>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Los lapachos</t>
+        </is>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>2</v>
@@ -34240,7 +34209,7 @@
         <v>10053</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K10" s="1" t="str">
         <f>A10&amp;","&amp;"'"&amp;B10&amp;"'"&amp;","&amp;"'"&amp;C10&amp;"'"&amp;","&amp;"'"&amp;D10&amp;"'"&amp;","&amp;"'"&amp;E10&amp;"'"&amp;","&amp;F10&amp;","&amp;G10&amp;","&amp;"'"&amp;H10&amp;"'"&amp;")"</f>
@@ -34249,11 +34218,11 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
         <f>J10&amp;K10&amp;";"</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.25">
@@ -34265,14 +34234,16 @@
           <t>Belen</t>
         </is>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>J. I. Rucci</t>
+        </is>
       </c>
       <c r="D11">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2</v>
@@ -34284,7 +34255,7 @@
         <v>10053</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K11" s="1" t="str">
         <f>A11&amp;","&amp;"'"&amp;B11&amp;"'"&amp;","&amp;"'"&amp;C11&amp;"'"&amp;","&amp;"'"&amp;D11&amp;"'"&amp;","&amp;"'"&amp;E11&amp;"'"&amp;","&amp;F11&amp;","&amp;G11&amp;","&amp;"'"&amp;H11&amp;"'"&amp;")"</f>
@@ -34293,11 +34264,11 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
         <f>J11&amp;K11&amp;";"</f>
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -34333,7 +34304,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
@@ -34351,10 +34322,10 @@
         </is>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -34392,7 +34363,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;"'"&amp;F2&amp;"'"&amp;","&amp;G2&amp;")"</f>
@@ -34401,11 +34372,11 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <f>J2&amp;K2&amp;";"</f>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.25">
@@ -34413,7 +34384,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
         <v>444</v>
@@ -34433,7 +34404,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1" t="str">
         <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;"'"&amp;F3&amp;"'"&amp;","&amp;G3&amp;")"</f>
@@ -34442,11 +34413,11 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.25">
@@ -34476,7 +34447,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K4" s="1" t="str">
         <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;"'"&amp;F4&amp;"'"&amp;","&amp;G4&amp;")"</f>
@@ -34485,11 +34456,11 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
         <f>J4&amp;K4&amp;";"</f>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.25">
@@ -34502,7 +34473,7 @@
         </is>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -34517,7 +34488,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="str">
         <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;"'"&amp;C6&amp;"'"&amp;","&amp;"'"&amp;D6&amp;"'"&amp;","&amp;"'"&amp;E6&amp;"'"&amp;","&amp;F6&amp;","&amp;"'"&amp;G6&amp;"'"&amp;")"</f>
@@ -34526,11 +34497,11 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
         <f>J6&amp;K6&amp;";"</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25">
@@ -34538,7 +34509,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>120</v>
@@ -34556,7 +34527,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1" t="str">
         <f>A7&amp;","&amp;"'"&amp;B7&amp;"'"&amp;","&amp;"'"&amp;C7&amp;"'"&amp;","&amp;"'"&amp;D7&amp;"'"&amp;","&amp;"'"&amp;E7&amp;"'"&amp;","&amp;F7&amp;","&amp;"'"&amp;G7&amp;"'"&amp;")"</f>
@@ -34565,11 +34536,11 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
         <f>J7&amp;K7&amp;";"</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="14.25">
@@ -34577,7 +34548,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>121</v>
@@ -34595,7 +34566,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K8" s="1" t="str">
         <f>A8&amp;","&amp;"'"&amp;B8&amp;"'"&amp;","&amp;"'"&amp;C8&amp;"'"&amp;","&amp;"'"&amp;D8&amp;"'"&amp;","&amp;"'"&amp;E8&amp;"'"&amp;","&amp;F8&amp;","&amp;"'"&amp;G8&amp;"'"&amp;")"</f>
@@ -34604,11 +34575,11 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
         <f>J8&amp;K8&amp;";"</f>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="14.25">
@@ -34621,7 +34592,7 @@
         </is>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -34636,7 +34607,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K9" s="1" t="str">
         <f>A9&amp;","&amp;"'"&amp;B9&amp;"'"&amp;","&amp;"'"&amp;C9&amp;"'"&amp;","&amp;"'"&amp;D9&amp;"'"&amp;","&amp;"'"&amp;E9&amp;"'"&amp;","&amp;F9&amp;","&amp;"'"&amp;G9&amp;"'"&amp;")"</f>
@@ -34645,11 +34616,11 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
         <f>J9&amp;K9&amp;";"</f>
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.25">
@@ -34662,7 +34633,7 @@
         </is>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -34677,7 +34648,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="str">
         <f>A10&amp;","&amp;"'"&amp;B10&amp;"'"&amp;","&amp;"'"&amp;C10&amp;"'"&amp;","&amp;"'"&amp;D10&amp;"'"&amp;","&amp;"'"&amp;E10&amp;"'"&amp;","&amp;F10&amp;","&amp;"'"&amp;G10&amp;"'"&amp;")"</f>
@@ -34686,11 +34657,11 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
         <f>J10&amp;K10&amp;";"</f>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.25">
@@ -34703,7 +34674,7 @@
         </is>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -34718,7 +34689,7 @@
         <v>6</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K11" s="1" t="str">
         <f>A11&amp;","&amp;"'"&amp;B11&amp;"'"&amp;","&amp;"'"&amp;C11&amp;"'"&amp;","&amp;"'"&amp;D11&amp;"'"&amp;","&amp;"'"&amp;E11&amp;"'"&amp;","&amp;F11&amp;","&amp;"'"&amp;G11&amp;"'"&amp;")"</f>
@@ -34727,19 +34698,16 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
         <f>J11&amp;K11&amp;";"</f>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="C12"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="J15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -34761,7 +34729,7 @@
   </sheetPr>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="75">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -34776,7 +34744,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
@@ -34784,7 +34752,7 @@
         </is>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
@@ -34825,7 +34793,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;C2&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;"'"&amp;E2&amp;"'"&amp;")"</f>
@@ -34834,11 +34802,11 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <f>J2&amp;K2&amp;";"</f>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14.25">
@@ -34864,7 +34832,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K3" s="1" t="str">
         <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;C3&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;"'"&amp;E3&amp;"'"&amp;")"</f>
@@ -34873,11 +34841,11 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.25">
@@ -34903,7 +34871,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K4" s="1" t="str">
         <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;C4&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;"'"&amp;E4&amp;"'"&amp;")"</f>
@@ -34912,11 +34880,11 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
         <f>J4&amp;K4&amp;";"</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.25">
@@ -34938,7 +34906,7 @@
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K6" s="1" t="str">
         <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;"'"&amp;C6&amp;"'"&amp;","&amp;D6&amp;","&amp;"'"&amp;E6&amp;"'"&amp;")"</f>
@@ -34947,11 +34915,11 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
         <f>J6&amp;K6&amp;";"</f>
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25">
@@ -34973,7 +34941,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="str">
         <f>A7&amp;","&amp;"'"&amp;B7&amp;"'"&amp;","&amp;"'"&amp;C7&amp;"'"&amp;","&amp;D7&amp;","&amp;"'"&amp;E7&amp;"'"&amp;")"</f>
@@ -34982,11 +34950,11 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
         <f>J7&amp;K7&amp;";"</f>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="14.25">
@@ -35008,7 +34976,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K8" s="1" t="str">
         <f>A8&amp;","&amp;"'"&amp;B8&amp;"'"&amp;","&amp;"'"&amp;C8&amp;"'"&amp;","&amp;D8&amp;","&amp;"'"&amp;E8&amp;"'"&amp;")"</f>
@@ -35017,11 +34985,11 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
         <f>J8&amp;K8&amp;";"</f>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="14.25">
@@ -35043,7 +35011,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K9" s="1" t="str">
         <f>A9&amp;","&amp;"'"&amp;B9&amp;"'"&amp;","&amp;"'"&amp;C9&amp;"'"&amp;","&amp;D9&amp;","&amp;"'"&amp;E9&amp;"'"&amp;")"</f>
@@ -35052,11 +35020,11 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
         <f>J9&amp;K9&amp;";"</f>
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.25">
@@ -35078,7 +35046,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K10" s="1" t="str">
         <f>A10&amp;","&amp;"'"&amp;B10&amp;"'"&amp;","&amp;"'"&amp;C10&amp;"'"&amp;","&amp;D10&amp;","&amp;"'"&amp;E10&amp;"'"&amp;")"</f>
@@ -35087,11 +35055,11 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
         <f>J10&amp;K10&amp;";"</f>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.25">
@@ -35113,7 +35081,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K11" s="1" t="str">
         <f>A11&amp;","&amp;"'"&amp;B11&amp;"'"&amp;","&amp;"'"&amp;C11&amp;"'"&amp;","&amp;D11&amp;","&amp;"'"&amp;E11&amp;"'"&amp;")"</f>
@@ -35122,11 +35090,11 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
         <f>J11&amp;K11&amp;";"</f>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>